<commit_message>
New test case - New customer page
</commit_message>
<xml_diff>
--- a/Guru99_Banking_Project/src/main/java/com/gurubanking/testdata/TestData2.xlsx
+++ b/Guru99_Banking_Project/src/main/java/com/gurubanking/testdata/TestData2.xlsx
@@ -75,7 +75,7 @@
     <t>Test12345</t>
   </si>
   <si>
-    <t>hjdh@hjs.com</t>
+    <t>ajdh@hjs.com</t>
   </si>
 </sst>
 </file>
@@ -453,7 +453,7 @@
   <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>